<commit_message>
Lista OGGETTI DA AGGIUNGERE scritta in Game.java.
</commit_message>
<xml_diff>
--- a/TextualAdventure/src/resources/Mappa.xlsx
+++ b/TextualAdventure/src/resources/Mappa.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="20115" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16650" windowHeight="6345"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,238 @@
     <sheet name="Foglio3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>LeaX_XIV</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Letto: dormendo cadi nel sonno verso sinistra.
+Libreria Sinistra: usando la chiave guadagni l'accesso a ???
+Libreria Destra</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Trono</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Libro: leggerlo sblocca il percorso per la Federazione dellEst</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Piccioni: lanciandogli un sasso volano via</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Parole Concatenate: vincendo quadagni la chiave della libreria</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Testa o Croce.
+"Fine" Avventura</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Si vede l'orologio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Morra Cinese</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LeaX_XIV:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Spawn Point.
+Sasso</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -58,13 +289,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -179,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -212,6 +456,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -554,7 +801,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="31" defaultRowHeight="49.5" customHeight="1"/>
@@ -579,7 +826,7 @@
       <c r="C3" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -625,6 +872,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>